<commit_message>
made changes in daily process
</commit_message>
<xml_diff>
--- a/Data/Bot1_Config.xlsx
+++ b/Data/Bot1_Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Finance Laptop\Documents\UiPath\Invoice Process Automation\DO and Invoice Process Automation_Bot 1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FE974E-B47B-40CD-8652-5A4761882EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47DC5AE-6A5F-4114-B1B0-A54CCE4EE229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12" yWindow="12" windowWidth="15336" windowHeight="8016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="343">
   <si>
     <t>Name</t>
   </si>
@@ -416,9 +416,6 @@
   </si>
   <si>
     <t>of Master htle where bot and user will save data</t>
-  </si>
-  <si>
-    <t>Email Body for sending Report for Daily Process</t>
   </si>
   <si>
     <t>Email Subject for sending Report for Consolidated Process</t>
@@ -930,15 +927,6 @@
     <t>Status Message for System Exception</t>
   </si>
   <si>
-    <t>C:\Users\Finance Laptop\Documents\UiPath\Invoice Process Automation\DO and Invoice Process Automation_Bot 1\Data\Input\ScheduleDetails_Bot1.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\Finance Laptop\Documents\UiPath\Invoice Process Automation\DO and Invoice Process Automation_Bot 1\Data\Input\</t>
-  </si>
-  <si>
-    <t>C:\Users\Finance Laptop\Documents\UiPath\Invoice Process Automation\DO and Invoice Process Automation_Bot 1\Exceptions_Screenshots\</t>
-  </si>
-  <si>
     <t>QuotationNumCol</t>
   </si>
   <si>
@@ -1096,6 +1084,27 @@
   </si>
   <si>
     <t>https://hhtc.insightservicing.sg/guest/login?return=%2F</t>
+  </si>
+  <si>
+    <t>Delay of 1 sec</t>
+  </si>
+  <si>
+    <t>Customer Entity column from Master file</t>
+  </si>
+  <si>
+    <t>invoicing@huphin.com.sg</t>
+  </si>
+  <si>
+    <t>Data\Input\ScheduleDetails_Bot1.xlsx</t>
+  </si>
+  <si>
+    <t>Email body for sending Report for daily Process</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots\</t>
+  </si>
+  <si>
+    <t>Data\Input\</t>
   </si>
 </sst>
 </file>
@@ -1491,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z982"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1587,7 +1596,7 @@
         <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>287</v>
+        <v>342</v>
       </c>
       <c r="C7" t="s">
         <v>113</v>
@@ -1598,7 +1607,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>288</v>
+        <v>341</v>
       </c>
       <c r="C8" t="s">
         <v>114</v>
@@ -1609,7 +1618,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>286</v>
+        <v>339</v>
       </c>
       <c r="C9" t="s">
         <v>115</v>
@@ -1620,7 +1629,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C10" t="s">
         <v>116</v>
@@ -1689,7 +1698,7 @@
         <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="25.2" customHeight="1">
@@ -1700,7 +1709,7 @@
         <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18.600000000000001" customHeight="1">
@@ -1711,7 +1720,7 @@
         <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1">
@@ -1722,7 +1731,7 @@
         <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
@@ -1733,7 +1742,7 @@
         <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -1744,7 +1753,7 @@
         <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -1752,10 +1761,10 @@
         <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -1766,7 +1775,7 @@
         <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -1777,7 +1786,7 @@
         <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
@@ -1785,10 +1794,10 @@
         <v>90</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
@@ -1799,7 +1808,7 @@
         <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
@@ -1810,7 +1819,7 @@
         <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="13.8" customHeight="1">
@@ -1821,7 +1830,7 @@
         <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
@@ -1832,7 +1841,7 @@
         <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
@@ -1843,7 +1852,7 @@
         <v>99</v>
       </c>
       <c r="C30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -1854,7 +1863,7 @@
         <v>98</v>
       </c>
       <c r="C31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
@@ -1865,7 +1874,7 @@
         <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
@@ -1876,7 +1885,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
@@ -1887,7 +1896,7 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
@@ -1898,7 +1907,7 @@
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
@@ -1909,7 +1918,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
@@ -1920,7 +1929,7 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
@@ -1931,7 +1940,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
@@ -1942,678 +1951,678 @@
         <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="C41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
+        <v>159</v>
+      </c>
+      <c r="B42" t="s">
         <v>160</v>
       </c>
-      <c r="B42" t="s">
-        <v>161</v>
-      </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B43">
         <v>0.5</v>
       </c>
       <c r="C43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C47" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C51" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
       <c r="A53" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C53" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
       <c r="A54" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C54" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1">
       <c r="A55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C55" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C56" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B57" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C57" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C58" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C59" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1">
       <c r="A60" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B60" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C60" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B61" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C61" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B62" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C62" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C63" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C64" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
+        <v>223</v>
+      </c>
+      <c r="B65" t="s">
         <v>224</v>
       </c>
-      <c r="B65" t="s">
-        <v>225</v>
-      </c>
       <c r="C65" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" t="s">
+        <v>221</v>
+      </c>
+      <c r="B66" t="s">
         <v>222</v>
       </c>
-      <c r="B66" t="s">
-        <v>223</v>
-      </c>
       <c r="C66" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B67" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C67" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1">
       <c r="A68" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B68" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C68" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1">
       <c r="A69" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B69" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C69" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1">
       <c r="A70" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B70" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C70" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1">
       <c r="A71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B71" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C71" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1">
       <c r="A72" t="s">
+        <v>219</v>
+      </c>
+      <c r="B72" t="s">
         <v>220</v>
       </c>
-      <c r="B72" t="s">
-        <v>221</v>
-      </c>
       <c r="C72" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1">
       <c r="A73" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B73" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C73" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1">
       <c r="A74" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C74" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C75" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1">
       <c r="A76" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C76" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1">
       <c r="A77" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C77" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1">
       <c r="A78" t="s">
+        <v>231</v>
+      </c>
+      <c r="B78" t="s">
         <v>232</v>
       </c>
-      <c r="B78" t="s">
-        <v>233</v>
-      </c>
       <c r="C78" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1">
       <c r="A79" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B79" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C79" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1">
       <c r="A80" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B80" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="14.25" customHeight="1">
       <c r="A81" t="s">
+        <v>276</v>
+      </c>
+      <c r="B81" t="s">
         <v>277</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>278</v>
-      </c>
-      <c r="C81" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="14.25" customHeight="1">
       <c r="A82" t="s">
+        <v>279</v>
+      </c>
+      <c r="B82" t="s">
         <v>280</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>281</v>
-      </c>
-      <c r="C82" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1">
       <c r="A83" t="s">
+        <v>282</v>
+      </c>
+      <c r="B83" t="s">
         <v>283</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>284</v>
-      </c>
-      <c r="C83" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1">
       <c r="A84" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B84" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C84" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1">
       <c r="A85" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B85" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C85" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1">
       <c r="A86" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B86" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C86" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1">
       <c r="A87" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B87" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C87" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1">
       <c r="A88" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B88" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C88" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1">
       <c r="A89" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B89" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C89" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1">
       <c r="A90" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B90" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C90" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="14.25" customHeight="1">
       <c r="A91" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B91" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C91" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.25" customHeight="1">
       <c r="A92" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1">
       <c r="A93" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B93">
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" customHeight="1">
       <c r="A94" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B94">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" customHeight="1">
       <c r="A95" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B95" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C95" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1">
       <c r="A96" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C96" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1">
       <c r="A97" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C97" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1">
       <c r="A98" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B98" t="s">
+        <v>326</v>
+      </c>
+      <c r="C98" t="s">
         <v>330</v>
-      </c>
-      <c r="C98" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1">
       <c r="A99" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B99" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C99" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B100" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C100" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1">
@@ -2621,21 +2630,21 @@
         <v>67</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C101" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1">
       <c r="A102" t="s">
         <v>58</v>
       </c>
-      <c r="B102" s="5" t="s">
-        <v>329</v>
+      <c r="B102" s="4" t="s">
+        <v>338</v>
       </c>
       <c r="C102" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1">
@@ -2643,10 +2652,10 @@
         <v>44</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C103" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1">
@@ -2654,10 +2663,10 @@
         <v>42</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C104" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1">
@@ -2668,22 +2677,28 @@
         <v>53</v>
       </c>
       <c r="C105" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1">
       <c r="A106" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B106">
         <v>1000</v>
       </c>
+      <c r="C106" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1">
       <c r="A107" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B107" t="s">
+        <v>333</v>
+      </c>
+      <c r="C107" t="s">
         <v>337</v>
       </c>
     </row>
@@ -3568,9 +3583,10 @@
     <hyperlink ref="B12" r:id="rId1" xr:uid="{AD309DEE-B8D8-4A7D-B651-869C229797D7}"/>
     <hyperlink ref="B103" r:id="rId2" xr:uid="{4F6F89CF-35F6-4E7B-85F3-078071B86125}"/>
     <hyperlink ref="B105" r:id="rId3" xr:uid="{C00EE444-5636-49D8-BBE8-AF4CFAF980A3}"/>
+    <hyperlink ref="B102" r:id="rId4" xr:uid="{A50C9DD0-9792-454A-8FE5-1DDE56BAFBE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -4742,8 +4758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B39A53-AEB2-4255-A0D4-3631566A9FD8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="B1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4770,7 +4786,7 @@
       </c>
       <c r="B2" s="7"/>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4779,7 +4795,7 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4787,7 +4803,7 @@
         <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4795,7 +4811,7 @@
         <v>94</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4803,7 +4819,7 @@
         <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>